<commit_message>
added ml bike prediction
</commit_message>
<xml_diff>
--- a/metric_learning_bicycle/experiments_ml.xlsx
+++ b/metric_learning_bicycle/experiments_ml.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YShimada-MBP16/Documents/Code_Github/DL_for_ImageData_and_Finetuning/metric_learning_bicycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271585F8-A7DB-BE46-9498-7EE3F2DACAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B08213-CAA5-934E-8581-9A23053B199B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="30160" windowHeight="17360" xr2:uid="{F453AF3D-8374-804C-B63E-8684ABA88DBC}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="30860" windowHeight="14920" xr2:uid="{F453AF3D-8374-804C-B63E-8684ABA88DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="LeaderBoard" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Round</t>
     <phoneticPr fontId="1"/>
@@ -120,6 +120,10 @@
   </si>
   <si>
     <t>ml-baseline</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ml-baseline2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -255,7 +259,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -285,6 +289,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,14 +682,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598F0E48-0E7C-6A47-B14E-8F6F7A14956C}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -784,6 +798,50 @@
       <c r="Q2" s="7"/>
       <c r="R2" s="8">
         <v>6.898148148148148E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="21">
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12">
+        <v>16</v>
+      </c>
+      <c r="F3" s="12">
+        <v>512</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="I3" s="12">
+        <v>5</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="12">
+        <v>512</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="12">
+        <v>45</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3">
+        <v>0.7611</v>
+      </c>
+      <c r="P3">
+        <v>0.75070000000000003</v>
+      </c>
+      <c r="R3" s="11">
+        <v>4.3750000000000004E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>